<commit_message>
NLP sms spam detector project
</commit_message>
<xml_diff>
--- a/Algorithm_and_projects.xlsx
+++ b/Algorithm_and_projects.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Regression" sheetId="1" r:id="rId1"/>
     <sheet name="Classification" sheetId="2" r:id="rId2"/>
-    <sheet name="Projects" sheetId="3" r:id="rId3"/>
+    <sheet name="NLP" sheetId="4" r:id="rId3"/>
+    <sheet name="Projects" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
   <si>
     <t>Sno.</t>
   </si>
@@ -124,14 +125,95 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>Loan Prediction 3</t>
+  </si>
+  <si>
+    <t>SMS spam/ham Detector</t>
+  </si>
+  <si>
+    <t>Yelp review</t>
+  </si>
+  <si>
+    <t>Udemy Python for Data Science and Machine Learning Bootcamp(22 hrs)</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Udemy Machine Learning A-Z Hands(41 hrs)</t>
+  </si>
+  <si>
+    <t>Restaurant_review</t>
+  </si>
+  <si>
+    <t>BOW</t>
+  </si>
+  <si>
+    <t>Competion</t>
+  </si>
+  <si>
+    <t>accuracy</t>
+  </si>
+  <si>
+    <t>analyticsvidhya.com</t>
+  </si>
+  <si>
+    <t>Aug 26 2018</t>
+  </si>
+  <si>
+    <t>Submission Date</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>naive_bayes(MultinomialNB)</t>
+  </si>
+  <si>
+    <t>Algorithm</t>
+  </si>
+  <si>
+    <t>/sms_spam_detector/notebooks/NLP (Natural Language Processing) with Python.ipynb</t>
+  </si>
+  <si>
+    <t>folder</t>
+  </si>
+  <si>
+    <t>Desc</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>30 Aaug 2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -147,7 +229,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -155,15 +237,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -221,7 +326,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -256,7 +361,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -468,7 +573,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,8 +740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,63 +872,209 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="66" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="H2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
+        <v>42</v>
+      </c>
+      <c r="E4" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.78472222222222199</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
auto summarize project and NLP folder sync
</commit_message>
<xml_diff>
--- a/Algorithm_and_projects.xlsx
+++ b/Algorithm_and_projects.xlsx
@@ -13,6 +13,7 @@
     <sheet name="Projects" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -275,9 +276,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -875,7 +873,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>